<commit_message>
integrated allocation algo with database
</commit_message>
<xml_diff>
--- a/somedata.xlsx
+++ b/somedata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6003F2-0930-4867-A5A4-EED5107CD0E2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293A25B5-FEFF-42A3-91B7-6113A8B53844}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{545FE80B-02C6-4C0D-8784-416F53C454F8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="8">
   <si>
     <t>Project Name</t>
   </si>
@@ -48,28 +48,13 @@
     <t>In Campus Centre?</t>
   </si>
   <si>
-    <t>This</t>
-  </si>
-  <si>
-    <t>That</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>Bad</t>
-  </si>
-  <si>
-    <t>Pro</t>
-  </si>
-  <si>
-    <t>Help</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>Industry</t>
   </si>
 </sst>
 </file>
@@ -421,15 +406,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5722D427-E56D-4A4D-A099-7E5EFC806B94}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="24" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -445,25 +433,31 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -471,81 +465,456 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>501</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>7</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>